<commit_message>
bugfix: json fileupload, extended: help messages
</commit_message>
<xml_diff>
--- a/documents/zeitaufzeichnung/michael_hauser-Zeitaufzeichnung.xlsx
+++ b/documents/zeitaufzeichnung/michael_hauser-Zeitaufzeichnung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="74">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t xml:space="preserve">Userhub Bugfixes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to other users Check other Userprofils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.052021</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -511,14 +517,14 @@
   <dimension ref="A1:D1006"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="E64" activeCellId="0" sqref="E64"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="C65" activeCellId="0" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0859375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.6"/>
@@ -1392,21 +1398,41 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="7"/>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="n">
+        <v>44344</v>
+      </c>
+      <c r="B63" s="5" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="7"/>
+      <c r="A64" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="9" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4"/>
-      <c r="B65" s="9"/>
+      <c r="A65" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B65" s="9" t="n">
+        <v>0.0208333333333333</v>
+      </c>
       <c r="C65" s="6"/>
       <c r="D65" s="7"/>
     </row>
@@ -7085,17 +7111,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0859375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7127,7 +7153,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7135,7 +7161,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7151,7 +7177,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>